<commit_message>
Implemented MYSQL ilo SQLLite
</commit_message>
<xml_diff>
--- a/static/downloads/logs.xlsx
+++ b/static/downloads/logs.xlsx
@@ -14,12 +14,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>2023-07-04</t>
-  </si>
-  <si>
-    <t>14:10:43</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="11">
+  <si>
+    <t>2023-07-20</t>
+  </si>
+  <si>
+    <t>08:38:26</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>test surname</t>
+  </si>
+  <si>
+    <t>marc.geraerts@uhasselt.be</t>
+  </si>
+  <si>
+    <t>lucp2284</t>
+  </si>
+  <si>
+    <t>08:44:59</t>
+  </si>
+  <si>
+    <t>08:47:45</t>
+  </si>
+  <si>
+    <t>08:51:44</t>
+  </si>
+  <si>
+    <t>08:53:36</t>
+  </si>
+  <si>
+    <t>08:59:31</t>
   </si>
 </sst>
 </file>
@@ -351,13 +378,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:C2"/>
+  <dimension ref="A2:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>1</v>
       </c>
@@ -366,6 +393,156 @@
       </c>
       <c r="C2" t="s">
         <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" t="s">
+        <v>4</v>
+      </c>
+      <c r="G8" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ready for deployment 22sep
</commit_message>
<xml_diff>
--- a/static/downloads/logs.xlsx
+++ b/static/downloads/logs.xlsx
@@ -14,39 +14,45 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="11">
-  <si>
-    <t>2023-07-20</t>
-  </si>
-  <si>
-    <t>08:38:26</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+  <si>
+    <t>2023-09-22</t>
+  </si>
+  <si>
+    <t>08:36:53</t>
+  </si>
+  <si>
+    <t>Marc</t>
+  </si>
+  <si>
+    <t>Geraerts</t>
+  </si>
+  <si>
+    <t>marc.geraerts@uhasselt.be</t>
+  </si>
+  <si>
+    <t>Lucp2284</t>
+  </si>
+  <si>
+    <t>09:55:44</t>
+  </si>
+  <si>
+    <t>test66</t>
   </si>
   <si>
     <t>test</t>
   </si>
   <si>
-    <t>test surname</t>
-  </si>
-  <si>
-    <t>marc.geraerts@uhasselt.be</t>
-  </si>
-  <si>
-    <t>lucp2284</t>
-  </si>
-  <si>
-    <t>08:44:59</t>
-  </si>
-  <si>
-    <t>08:47:45</t>
-  </si>
-  <si>
-    <t>08:51:44</t>
-  </si>
-  <si>
-    <t>08:53:36</t>
-  </si>
-  <si>
-    <t>08:59:31</t>
+    <t>lucp7894</t>
+  </si>
+  <si>
+    <t>test66@test.com</t>
+  </si>
+  <si>
+    <t>09:56:06</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -378,7 +384,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:G8"/>
+  <dimension ref="A2:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -418,16 +424,16 @@
         <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F3" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="G3" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -438,111 +444,19 @@
         <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="G4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F5" t="s">
-        <v>4</v>
-      </c>
-      <c r="G5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E6" t="s">
-        <v>3</v>
-      </c>
-      <c r="F6" t="s">
-        <v>4</v>
-      </c>
-      <c r="G6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E7" t="s">
-        <v>3</v>
-      </c>
-      <c r="F7" t="s">
-        <v>4</v>
-      </c>
-      <c r="G7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>0</v>
-      </c>
-      <c r="C8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" t="s">
-        <v>2</v>
-      </c>
-      <c r="E8" t="s">
-        <v>3</v>
-      </c>
-      <c r="F8" t="s">
-        <v>4</v>
-      </c>
-      <c r="G8" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>